<commit_message>
add new exercises, section, fix typo, update anki deck/word list
- fixed some typos in lesson-9/literacy-8. (2nd ed.)
- updated anki deck and word list for lesson 9. (3rd ed.)
- added new section for lesson 10. (3rd ed.)
- added the following exercises.

# Lesson 9 (3rd ed.)
- Reading Practice: ソラさんの日記
- Useful Expressions: for Mail/Letters
- Workbook: Kanji Writing Practice
- Workbook: Using Kanji
</commit_message>
<xml_diff>
--- a/resources/tools/wordlist_E-J/lessons-3rd/lesson-9.xlsx
+++ b/resources/tools/wordlist_E-J/lessons-3rd/lesson-9.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B140"/>
+  <dimension ref="A1:B145"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1360,742 +1360,802 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>A.M.</t>
+          <t>Thank you for everything.</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>午前|ごぜん</t>
+          <t>いろいろおせわになりました。</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>P.M.; in the afternoon</t>
+          <t>Please take care of yourself.</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>午後|ごご</t>
+          <t>体に気をつけてください。|からだにきをつけてください。</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>in the morning</t>
+          <t>I am looking forward to seeing you.</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>午前中|ごぜんちゅう</t>
+          <t>お会いできるのを楽しみにしています。|おあいできるをたのしみにしています。</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>noon</t>
+          <t>Congratulations on...</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>正午|しょうご</t>
+          <t>～おめでとう（ございます）。</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>after...</t>
+          <t>Happy Birthday.</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>～の後|～のあと</t>
+          <t>（お）たんじょうびおめでとう。</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>later</t>
+          <t>A.M.</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>後で|あとで</t>
+          <t>午前|ごぜん</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>back; behind</t>
+          <t>P.M.; in the afternoon</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>後ろ|うしろ</t>
+          <t>午後|ごご</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>lastly</t>
+          <t>in the morning</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>最後に|さいごに</t>
+          <t>午前中|ごぜんちゅう</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>before; front</t>
+          <t>noon</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>前|まえ</t>
+          <t>正午|しょうご</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>after...</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>名前|なまえ</t>
+          <t>～の後|～のあと</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>advance sale</t>
+          <t>later</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>前売り|まえうり</t>
+          <t>後で|あとで</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>back; behind</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>名前|なまえ</t>
+          <t>後ろ|うしろ</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>famous</t>
+          <t>lastly</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>有名な|ゆうめいな</t>
+          <t>最後に|さいごに</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>name card</t>
+          <t>before; front</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>名刺|めいし</t>
+          <t>前|まえ</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>full name</t>
+          <t>name</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>氏名|しめい</t>
+          <t>名前|なまえ</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>family name</t>
+          <t>advance sale</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>名字|みょうじ</t>
+          <t>前売り|まえうり</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>white</t>
+          <t>name</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>白い|しろい</t>
+          <t>名前|なまえ</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>blank sheet</t>
+          <t>famous</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>白紙|はくし</t>
+          <t>有名な|ゆうめいな</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>white color</t>
+          <t>name card</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>白|しろ</t>
+          <t>名刺|めいし</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>swan</t>
+          <t>full name</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>白鳥|はくちょう</t>
+          <t>氏名|しめい</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>rain</t>
+          <t>family name</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>雨|あめ</t>
+          <t>名字|みょうじ</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>rainy season</t>
+          <t>white</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>雨期|うき</t>
+          <t>白い|しろい</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>rainy season (East Asia)</t>
+          <t>blank sheet</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>梅雨|つゆ</t>
+          <t>白紙|はくし</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>heavy rain</t>
+          <t>white color</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>大雨|おおあめ</t>
+          <t>白|しろ</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>to write</t>
+          <t>swan</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>書く|かく</t>
+          <t>白鳥|はくちょう</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>dictionary</t>
+          <t>rain</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>辞書|じしょ</t>
+          <t>雨|あめ</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>textbook</t>
+          <t>rainy season</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>教科書|きょうかしょ</t>
+          <t>雨期|うき</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>library</t>
+          <t>rainy season (East Asia)</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>図書館|としょかん</t>
+          <t>梅雨|つゆ</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>friend</t>
+          <t>heavy rain</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>友だち|ともだち</t>
+          <t>大雨|おおあめ</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>best friend</t>
+          <t>to write</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>親友|しんゆう</t>
+          <t>書く|かく</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>friend (formal)</t>
+          <t>dictionary</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>友人|ゆうじん</t>
+          <t>辞書|じしょ</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>friendship</t>
+          <t>textbook</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>友情|ゆうじょう</t>
+          <t>教科書|きょうかしょ</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>time</t>
+          <t>library</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>時間|じかん</t>
+          <t>図書館|としょかん</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>two hours</t>
+          <t>friend</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>二時間|にじかん</t>
+          <t>友だち|ともだち</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>between</t>
+          <t>best friend</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>間|あいだ</t>
+          <t>親友|しんゆう</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>human being</t>
+          <t>friend (formal)</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>人間|にんげん</t>
+          <t>友人|ゆうじん</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>one week</t>
+          <t>friendship</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>一週間|いっしゅうかん</t>
+          <t>友情|ゆうじょう</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>house</t>
+          <t>time</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>家|いえ</t>
+          <t>時間|じかん</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>family</t>
+          <t>two hours</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>家族|かぞく</t>
+          <t>二時間|にじかん</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>house; home</t>
+          <t>between</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>家|うち</t>
+          <t>間|あいだ</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>my wife</t>
+          <t>human being</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>家内|かない</t>
+          <t>人間|にんげん</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>author</t>
+          <t>one week</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>作家|さっか</t>
+          <t>一週間|いっしゅうかん</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>to speak</t>
+          <t>house</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>話す|はなす</t>
+          <t>家|いえ</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>talk; story</t>
+          <t>family</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>話|はなし</t>
+          <t>家族|かぞく</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>telephone</t>
+          <t>house; home</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>電話|でんわ</t>
+          <t>家|うち</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>conversation</t>
+          <t>my wife</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>会話|かいわ</t>
+          <t>家内|かない</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>little</t>
+          <t>author</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>少し|すこし</t>
+          <t>作家|さっか</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>few</t>
+          <t>to speak</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>少ない|すくない</t>
+          <t>話す|はなす</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>a little</t>
+          <t>talk; story</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>少々|しょうしょう</t>
+          <t>話|はなし</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>girl</t>
+          <t>telephone</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>少女|しょうじょ</t>
+          <t>電話|でんわ</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>boy</t>
+          <t>conversation</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>少年|しょうねん</t>
+          <t>会話|かいわ</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>old (for things)</t>
+          <t>little</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>古い|ふるい</t>
+          <t>少し|すこし</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>secondhand</t>
+          <t>few</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>中古|ちゅうこ</t>
+          <t>少ない|すくない</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>ancient times</t>
+          <t>a little</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>古代|こだい</t>
+          <t>少々|しょうしょう</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>to know</t>
+          <t>girl</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>知る|しる</t>
+          <t>少女|しょうじょ</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>acquaintance (formal)</t>
+          <t>boy</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>知人|ちじん</t>
+          <t>少年|しょうねん</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>acquaintance</t>
+          <t>old (for things)</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>知り合い|しりあい</t>
+          <t>古い|ふるい</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>to come</t>
+          <t>secondhand</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>来る|くる</t>
+          <t>中古|ちゅうこ</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>to come (long-form)</t>
+          <t>ancient times</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>来ます|きます</t>
+          <t>古代|こだい</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>not to come</t>
+          <t>to know</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>来ない|こない</t>
+          <t>知る|しる</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>next week</t>
+          <t>acquaintance (formal)</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>来週|らいしゅう</t>
+          <t>知人|ちじん</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
+          <t>acquaintance</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>知り合い|しりあい</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>to come</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>来る|くる</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>to come (long-form)</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>来ます|きます</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>not to come</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>来ない|こない</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>next week</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>来週|らいしゅう</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
           <t>visit to Japan</t>
         </is>
       </c>
-      <c r="B140" t="inlineStr">
+      <c r="B145" t="inlineStr">
         <is>
           <t>来日|らいにち</t>
         </is>

</xml_diff>